<commit_message>
Added validation for 'NoContainerHistory'
</commit_message>
<xml_diff>
--- a/sht2.xlsx
+++ b/sht2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <x:si>
     <x:t>Action</x:t>
   </x:si>
@@ -122,241 +122,208 @@
     <x:t>unchecked</x:t>
   </x:si>
   <x:si>
-    <x:t>21063927</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FLTZ454726</x:t>
+    <x:t>21069510</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FLXZ442171</x:t>
   </x:si>
   <x:si>
     <x:t>BACP</x:t>
   </x:si>
   <x:si>
-    <x:t>BAUI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BBUN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HLBU908993</x:t>
+    <x:t>BATRA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>APYK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DFSU619759</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FO - Full Out</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31-Jul-2023 22:22:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HPL</x:t>
   </x:si>
   <x:si>
     <x:t>E</x:t>
   </x:si>
   <x:si>
-    <x:t>O</x:t>
+    <x:t>MISSING INGATE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OAKLAND</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A. P. TRUCKING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TRAPACI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IZ1230571084</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Y</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-Dec-2021 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EDITRG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-Aug-2023 15:28:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EDI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19745137</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BAUP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAAU539502</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19-Apr-2023 13:04:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAPAG LLOYD AMERICA LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67214098</x:t>
+  </x:si>
+  <x:si>
+    <x:t>610625851</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20-Apr-2023 05:00:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>acano@flexivan.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:57:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19716905</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RESP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>I</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BI - Bare In</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 14:11:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FVIU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RED SEA EXPRESS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18-Apr-2023 05:00:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19716134</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ONEU910846</x:t>
   </x:si>
   <x:si>
     <x:t>EO - Empty Out</x:t>
   </x:si>
   <x:si>
-    <x:t>31-Jul-2023 13:28:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HPL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HLCU</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MISSING INGATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Oakland</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BBS TRUCKING INC.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>USOAKNWDA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>61234786</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Y</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01-Dec-2021 00:00:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EDITRG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01-Aug-2023 15:28:28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EDI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20922806</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BATRA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RESP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ONEU902061</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19-Jul-2023 14:02:00</x:t>
+    <x:t>17-Apr-2023 13:32:00</x:t>
   </x:si>
   <x:si>
     <x:t>ONEY</x:t>
   </x:si>
   <x:si>
-    <x:t>LT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OAKLAND</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RED SEA EXPRESS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRAPACI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23297458S001</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20-Jul-2023 05:00:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>brodriguez@flexivan.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26-Jul-2023 14:00:24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21003688</x:t>
-  </x:si>
-  <x:si>
-    <x:t>B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>I</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BI - Bare In</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19-Jul-2023 10:56:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26-Jul-2023 14:00:19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20920365</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MORU112670</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19-Jul-2023 10:46:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21003687</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19-Jul-2023 08:10:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26-Jul-2023 13:59:56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20917858</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MORU110589</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19-Jul-2023 07:58:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20990647</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RXPP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HLBU215696</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EI - Empty In</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18-Jul-2023 12:59:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RELIABLE EXPRESS TRANSPORTATION INC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>69900367</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26-Jul-2023 05:00:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20878572</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHPTR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FO - Full Out</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17-Jul-2023 12:06:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OAKLAND, CA USA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SSOFA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SGN230524817</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18-Jul-2023 05:00:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20805175</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHPO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FI - Full In</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12-Jul-2023 00:19:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHIPPER TRANSPORT EXPRESS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12-Jul-2023 05:00:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20805014</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BA58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12-Jul-2023 00:03:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHIPPERS TRANSPORT EXPRESS</x:t>
+    <x:t>23167458S001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19792477</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 13:22:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:57:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19715154</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAIU568171</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 11:43:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19792474</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 11:33:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:56:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19714056</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZLU911590</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 10:38:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19792470</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 10:28:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:56:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19712646</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEGU918786</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 09:12:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -877,9 +844,6 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="M2" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
         <x:v>44</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
@@ -897,10 +861,7 @@
       <x:c r="T2" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="U2" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="W2" s="0" t="s">
+      <x:c r="X2" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="s">
@@ -942,10 +903,10 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
         <x:v>58</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>59</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
         <x:v>39</x:v>
@@ -957,28 +918,40 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="N3" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="L3" s="0" t="s">
+      <x:c r="P3" s="0" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="M3" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="P3" s="0" t="s">
+      <x:c r="Q3" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R3" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="T3" s="0" t="s">
         <x:v>62</x:v>
       </x:c>
-      <x:c r="Q3" s="0" t="s">
+      <x:c r="U3" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="V3" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="W3" s="0" t="s">
         <x:v>63</x:v>
       </x:c>
-      <x:c r="R3" s="0" t="s">
+      <x:c r="X3" s="0" t="s">
         <x:v>64</x:v>
-      </x:c>
-      <x:c r="T3" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="W3" s="0" t="s">
-        <x:v>66</x:v>
       </x:c>
       <x:c r="Z3" s="0" t="s">
         <x:v>51</x:v>
@@ -993,13 +966,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="AD3" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="AE3" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AF3" s="0" t="s">
         <x:v>67</x:v>
-      </x:c>
-      <x:c r="AE3" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="AF3" s="0" t="s">
-        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -1007,7 +980,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>34</x:v>
@@ -1019,31 +992,37 @@
         <x:v>57</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="I4" s="0" t="s">
+      <x:c r="J4" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="J4" s="0" t="s">
+      <x:c r="K4" s="0" t="s">
         <x:v>73</x:v>
       </x:c>
-      <x:c r="K4" s="0" t="s">
+      <x:c r="L4" s="0" t="s">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="L4" s="0" t="s">
+      <x:c r="M4" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P4" s="0" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="M4" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="P4" s="0" t="s">
+      <x:c r="Q4" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R4" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="T4" s="0" t="s">
         <x:v>62</x:v>
-      </x:c>
-      <x:c r="W4" s="0" t="s">
-        <x:v>66</x:v>
       </x:c>
       <x:c r="Z4" s="0" t="s">
         <x:v>51</x:v>
@@ -1055,16 +1034,16 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="AC4" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD4" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE4" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AF4" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:32" x14ac:dyDescent="0.35">
@@ -1072,7 +1051,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>34</x:v>
@@ -1081,46 +1060,46 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="J5" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K5" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="L5" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M5" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P5" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="Q5" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="R5" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="T5" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="W5" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z5" s="0" t="s">
         <x:v>51</x:v>
@@ -1135,13 +1114,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="AD5" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="AE5" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AF5" s="0" t="s">
         <x:v>67</x:v>
-      </x:c>
-      <x:c r="AE5" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="AF5" s="0" t="s">
-        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:32" x14ac:dyDescent="0.35">
@@ -1149,7 +1128,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>79</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>34</x:v>
@@ -1158,34 +1137,34 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
         <x:v>71</x:v>
       </x:c>
-      <x:c r="I6" s="0" t="s">
+      <x:c r="J6" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="J6" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>80</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="L6" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M6" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P6" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="W6" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z6" s="0" t="s">
         <x:v>51</x:v>
@@ -1197,16 +1176,16 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="AC6" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AD6" s="0" t="s">
-        <x:v>81</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="AE6" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF6" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -1214,7 +1193,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>82</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>34</x:v>
@@ -1223,46 +1202,46 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>83</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="L7" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M7" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P7" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="Q7" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="R7" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="T7" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="W7" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z7" s="0" t="s">
         <x:v>51</x:v>
@@ -1277,13 +1256,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="AD7" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="AE7" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AF7" s="0" t="s">
         <x:v>67</x:v>
-      </x:c>
-      <x:c r="AE7" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="AF7" s="0" t="s">
-        <x:v>69</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:32" x14ac:dyDescent="0.35">
@@ -1291,7 +1270,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>34</x:v>
@@ -1300,46 +1279,34 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>86</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="J8" s="0" t="s">
-        <x:v>88</x:v>
-      </x:c>
       <x:c r="K8" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="L8" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M8" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P8" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="Q8" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="R8" s="0" t="s">
-        <x:v>90</x:v>
-      </x:c>
-      <x:c r="T8" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="W8" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z8" s="0" t="s">
         <x:v>51</x:v>
@@ -1351,16 +1318,16 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="AC8" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AD8" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="AE8" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF8" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:32" x14ac:dyDescent="0.35">
@@ -1368,7 +1335,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>34</x:v>
@@ -1377,46 +1344,46 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="J9" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K9" s="0" t="s">
-        <x:v>97</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="L9" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M9" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P9" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="Q9" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="R9" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="T9" s="0" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="X9" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="W9" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z9" s="0" t="s">
         <x:v>51</x:v>
@@ -1431,13 +1398,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="AD9" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE9" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF9" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -1445,7 +1412,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>34</x:v>
@@ -1454,46 +1421,34 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="G10" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
         <x:v>72</x:v>
       </x:c>
-      <x:c r="J10" s="0" t="s">
-        <x:v>104</x:v>
-      </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="L10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M10" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P10" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="Q10" s="0" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="R10" s="0" t="s">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="T10" s="0" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="X10" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="W10" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z10" s="0" t="s">
         <x:v>51</x:v>
@@ -1505,16 +1460,16 @@
         <x:v>52</x:v>
       </x:c>
       <x:c r="AC10" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AD10" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="AE10" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF10" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:32" x14ac:dyDescent="0.35">
@@ -1522,7 +1477,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>34</x:v>
@@ -1531,46 +1486,46 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>87</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>95</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K11" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="L11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M11" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
       <x:c r="P11" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="Q11" s="0" t="s">
-        <x:v>98</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="R11" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="T11" s="0" t="s">
-        <x:v>99</x:v>
-      </x:c>
-      <x:c r="X11" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="W11" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z11" s="0" t="s">
         <x:v>51</x:v>
@@ -1585,13 +1540,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="AD11" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE11" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF11" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added Code for Act Loc
</commit_message>
<xml_diff>
--- a/sht2.xlsx
+++ b/sht2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <x:si>
     <x:t>Action</x:t>
   </x:si>
@@ -122,10 +122,10 @@
     <x:t>unchecked</x:t>
   </x:si>
   <x:si>
-    <x:t>21067960</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FVXZ177262</x:t>
+    <x:t>21069510</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FLXZ442171</x:t>
   </x:si>
   <x:si>
     <x:t>BACP</x:t>
@@ -134,244 +134,196 @@
     <x:t>BATRA</x:t>
   </x:si>
   <x:si>
-    <x:t>SIDO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FANU316326</x:t>
+    <x:t>APYK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DFSU619759</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>O</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FO - Full Out</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31-Jul-2023 22:22:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HPL</x:t>
   </x:si>
   <x:si>
     <x:t>E</x:t>
   </x:si>
   <x:si>
+    <x:t>MISSING INGATE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OAKLAND</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A. P. TRUCKING</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TRAPACI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IZ1230571084</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Y</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-Dec-2021 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EDITRG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01-Aug-2023 15:28:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EDI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19745137</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BAUP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAAU539502</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19-Apr-2023 13:04:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAPAG LLOYD AMERICA LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>67214098</x:t>
+  </x:si>
+  <x:si>
+    <x:t>610625851</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20-Apr-2023 05:00:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>acano@flexivan.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:57:28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19716905</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RESP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>B</x:t>
+  </x:si>
+  <x:si>
     <x:t>I</x:t>
   </x:si>
   <x:si>
-    <x:t>EI - Empty In</x:t>
-  </x:si>
-  <x:si>
-    <x:t>31-Jul-2023 19:01:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HPL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PREV ACT ERROR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OAKLAND</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SEAPORT INTERMODAL INC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRAPACI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Y</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01-Dec-2021 00:00:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EDITRG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>01-Aug-2023 15:28:28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EDI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21062998</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BAUP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>O</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FO - Full Out</x:t>
-  </x:si>
-  <x:si>
-    <x:t>31-Jul-2023 11:47:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INTERDOM LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MISSING INGATE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4586418</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21019707</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BA58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KAML</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CICU411313</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26-Jul-2023 19:17:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HYUND</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OAKLAND, CA USA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KAMAL TRUCKING CORPORATION</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SSOFA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SHAZ98232500</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27-Jul-2023 05:00:02</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20994440</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ITCM</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UACU531129</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FI - Full In</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25-Jul-2023 10:50:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PHWC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INTELLIGENT TRANSPORTATION CORPORAT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7570410121</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26-Jul-2023 05:00:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20977416</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24-Jul-2023 15:51:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INTELLIGENT TRANSPORTATION CORPORATION</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HAM2305BBZU7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25-Jul-2023 05:00:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20976173</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RXPP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRHU487863</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24-Jul-2023 14:31:00</x:t>
+    <x:t>BI - Bare In</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 14:11:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FVIU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RED SEA EXPRESS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18-Apr-2023 05:00:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19716134</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ONEU910846</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EO - Empty Out</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 13:32:00</x:t>
   </x:si>
   <x:si>
     <x:t>ONEY</x:t>
   </x:si>
   <x:si>
-    <x:t>RELIABLE EXPRESS TRANSPORTATION INC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20936420</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20-Jul-2023 14:44:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NB3BH4224500</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21-Jul-2023 05:00:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>brodriguez@flexivan.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21-Jul-2023 11:32:56</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20933802</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AUZG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BSIU820921</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20-Jul-2023 11:17:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ARAUZ TRUCKING LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>66233880</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20895505</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EO - Empty Out</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17-Jul-2023 13:24:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>19-Jul-2023 05:00:01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20895396</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IMPC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HLBU178885</x:t>
-  </x:si>
-  <x:si>
-    <x:t>17-Jul-2023 10:34:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IMPACT TRANSPORTATION, LLC</x:t>
+    <x:t>23167458S001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19792477</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 13:22:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:57:18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19715154</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAIU568171</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 11:43:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19792474</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 11:33:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:56:59</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19714056</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SZLU911590</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 10:38:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19792470</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 10:28:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24-Apr-2023 08:56:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19712646</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEGU918786</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-Apr-2023 09:12:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -892,43 +844,46 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="M2" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="O2" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="P2" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="Q2" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="R2" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="T2" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="X2" s="0" t="s">
+        <x:v>50</x:v>
       </x:c>
       <x:c r="Z2" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA2" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB2" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC2" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD2" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="AE2" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="AF2" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:32" x14ac:dyDescent="0.35">
@@ -936,7 +891,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>34</x:v>
@@ -945,22 +900,22 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
         <x:v>59</x:v>
@@ -969,25 +924,22 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="M3" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="N3" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="O3" s="0" t="s">
+      <x:c r="P3" s="0" t="s">
         <x:v>61</x:v>
       </x:c>
-      <x:c r="P3" s="0" t="s">
+      <x:c r="Q3" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R3" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="T3" s="0" t="s">
         <x:v>62</x:v>
-      </x:c>
-      <x:c r="Q3" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="R3" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="T3" s="0" t="s">
-        <x:v>63</x:v>
       </x:c>
       <x:c r="U3" s="0" t="s">
         <x:v>60</x:v>
@@ -995,29 +947,32 @@
       <x:c r="V3" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
+      <x:c r="W3" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
       <x:c r="X3" s="0" t="s">
         <x:v>64</x:v>
       </x:c>
       <x:c r="Z3" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA3" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB3" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC3" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD3" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="AE3" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF3" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:32" x14ac:dyDescent="0.35">
@@ -1025,7 +980,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>34</x:v>
@@ -1034,67 +989,61 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="K4" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="L4" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="M4" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="P4" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="Q4" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="R4" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="T4" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="X4" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Z4" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA4" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB4" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC4" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD4" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE4" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
       <x:c r="AF4" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:32" x14ac:dyDescent="0.35">
@@ -1102,7 +1051,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>34</x:v>
@@ -1111,16 +1060,16 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
         <x:v>78</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
         <x:v>40</x:v>
@@ -1135,43 +1084,43 @@
         <x:v>81</x:v>
       </x:c>
       <x:c r="M5" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P5" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Q5" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R5" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="T5" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="P5" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q5" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="R5" s="0" t="s">
+      <x:c r="W5" s="0" t="s">
         <x:v>82</x:v>
       </x:c>
-      <x:c r="T5" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="W5" s="0" t="s">
-        <x:v>83</x:v>
-      </x:c>
       <x:c r="Z5" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA5" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB5" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC5" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD5" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE5" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF5" s="0" t="s">
-        <x:v>84</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:32" x14ac:dyDescent="0.35">
@@ -1179,7 +1128,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>85</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>34</x:v>
@@ -1191,64 +1140,52 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>77</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>78</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="J6" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="K6" s="0" t="s">
-        <x:v>86</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="L6" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M6" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="P6" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q6" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="R6" s="0" t="s">
-        <x:v>87</x:v>
-      </x:c>
-      <x:c r="T6" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="X6" s="0" t="s">
-        <x:v>88</x:v>
+      <x:c r="W6" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z6" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA6" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB6" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC6" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AD6" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="AE6" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF6" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -1256,7 +1193,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>90</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>34</x:v>
@@ -1268,61 +1205,64 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>91</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>92</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="J7" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K7" s="0" t="s">
-        <x:v>93</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="L7" s="0" t="s">
-        <x:v>94</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M7" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P7" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Q7" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R7" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="T7" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="P7" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q7" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="R7" s="0" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="T7" s="0" t="s">
-        <x:v>48</x:v>
+      <x:c r="W7" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z7" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA7" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB7" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC7" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD7" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE7" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF7" s="0" t="s">
-        <x:v>89</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:32" x14ac:dyDescent="0.35">
@@ -1330,7 +1270,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>96</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
         <x:v>34</x:v>
@@ -1342,64 +1282,52 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="K8" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="L8" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="M8" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P8" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="W8" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="Z8" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AA8" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AB8" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC8" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AD8" s="0" t="s">
         <x:v>91</x:v>
       </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>92</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="I8" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="J8" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="K8" s="0" t="s">
-        <x:v>97</x:v>
-      </x:c>
-      <x:c r="L8" s="0" t="s">
-        <x:v>94</x:v>
-      </x:c>
-      <x:c r="M8" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="P8" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q8" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="R8" s="0" t="s">
-        <x:v>95</x:v>
-      </x:c>
-      <x:c r="T8" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="X8" s="0" t="s">
-        <x:v>98</x:v>
-      </x:c>
-      <x:c r="Z8" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="AA8" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="AB8" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="AC8" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="AD8" s="0" t="s">
-        <x:v>99</x:v>
-      </x:c>
       <x:c r="AE8" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF8" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:32" x14ac:dyDescent="0.35">
@@ -1407,7 +1335,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>102</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>34</x:v>
@@ -1419,13 +1347,13 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>103</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
         <x:v>40</x:v>
@@ -1434,49 +1362,49 @@
         <x:v>79</x:v>
       </x:c>
       <x:c r="K9" s="0" t="s">
-        <x:v>105</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="L9" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M9" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P9" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Q9" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R9" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="T9" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="P9" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q9" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="R9" s="0" t="s">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="T9" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="W9" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z9" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA9" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB9" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC9" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD9" s="0" t="s">
-        <x:v>99</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE9" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF9" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:32" x14ac:dyDescent="0.35">
@@ -1484,7 +1412,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>108</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>34</x:v>
@@ -1496,64 +1424,52 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>103</x:v>
-      </x:c>
-      <x:c r="G10" s="0" t="s">
-        <x:v>104</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="J10" s="0" t="s">
-        <x:v>109</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="K10" s="0" t="s">
-        <x:v>110</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="L10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M10" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="P10" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q10" s="0" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="R10" s="0" t="s">
-        <x:v>106</x:v>
-      </x:c>
-      <x:c r="T10" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
       <x:c r="W10" s="0" t="s">
-        <x:v>107</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z10" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA10" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB10" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC10" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AD10" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="AE10" s="0" t="s">
-        <x:v>100</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF10" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:32" x14ac:dyDescent="0.35">
@@ -1561,7 +1477,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>112</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>34</x:v>
@@ -1573,61 +1489,64 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>113</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>114</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="K11" s="0" t="s">
-        <x:v>115</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="L11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="M11" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P11" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="Q11" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="R11" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="T11" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="P11" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="Q11" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="R11" s="0" t="s">
-        <x:v>116</x:v>
-      </x:c>
-      <x:c r="T11" s="0" t="s">
-        <x:v>48</x:v>
+      <x:c r="W11" s="0" t="s">
+        <x:v>82</x:v>
       </x:c>
       <x:c r="Z11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AA11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="AB11" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="AC11" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="AD11" s="0" t="s">
-        <x:v>111</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="AE11" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF11" s="0" t="s">
-        <x:v>101</x:v>
+        <x:v>67</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>